<commit_message>
aanpassing op updatelijst kaarthouders
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51059992\Adecco\NL Modis - RPA Consultancy - Interne processen\RPAProcessen\4.1 - NS_BusinessCards_Akkodis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF774936-2268-4CC8-AFDD-4CB866ACBBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CA432-EE3C-456A-B9FD-71402EB3DF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>NS_filepath_processingFolder</t>
-  </si>
-  <si>
-    <t>NS_filepath_factuurNS</t>
   </si>
   <si>
     <t>NS_filepath_rapportage</t>
@@ -624,7 +621,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -2810,7 +2807,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2889,14 +2886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>

</xml_diff>